<commit_message>
Commit for Fee Student concession
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/AdmissionReports.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/AdmissionReports.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635" firstSheet="35" activeTab="36"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635" firstSheet="33" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="IVRM_StaffLogin_Data" sheetId="7" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="44">
   <si>
     <t>Admission Number</t>
   </si>
@@ -173,13 +173,22 @@
   </si>
   <si>
     <t>2017-020</t>
+  </si>
+  <si>
+    <t>2018-058</t>
+  </si>
+  <si>
+    <t>2016-024</t>
+  </si>
+  <si>
+    <t>2017-047</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +217,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,6 +266,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1391,12 +1410,329 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1418,7 +1754,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -1429,84 +1765,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1523,254 +1790,8 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>40</v>
+      <c r="A2" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>

</xml_diff>